<commit_message>
Codes adjusted to styleguide
</commit_message>
<xml_diff>
--- a/20160919 MSE-ToDo Status.xlsx
+++ b/20160919 MSE-ToDo Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reiskemo.hub\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reiskemo.hub\Documents\GitHub\MSE-ToDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
   <si>
     <t>MSEedfnormal</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>description added acc. to book</t>
-  </si>
-  <si>
-    <t>author</t>
   </si>
   <si>
     <t>MSEperformance</t>
@@ -262,6 +259,18 @@
   </si>
   <si>
     <t>Qs not in the book but on GitHub</t>
+  </si>
+  <si>
+    <t>Code OK Styleguide?</t>
+  </si>
+  <si>
+    <t>Runs?</t>
+  </si>
+  <si>
+    <t>kredit.csv missing!</t>
+  </si>
+  <si>
+    <t>braucht extrem lang</t>
   </si>
 </sst>
 </file>
@@ -294,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +322,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -327,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -351,6 +366,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -632,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,15 +664,18 @@
     <col min="1" max="1" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -662,8 +686,17 @@
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -675,8 +708,12 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -690,8 +727,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -703,27 +742,37 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -735,92 +784,124 @@
         <v>10</v>
       </c>
       <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="F8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
@@ -829,28 +910,40 @@
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>5</v>
@@ -859,13 +952,15 @@
         <v>10</v>
       </c>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -874,13 +969,15 @@
         <v>10</v>
       </c>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>5</v>
@@ -889,64 +986,78 @@
         <v>10</v>
       </c>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>5</v>
@@ -955,13 +1066,15 @@
         <v>10</v>
       </c>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>5</v>
@@ -970,13 +1083,15 @@
         <v>10</v>
       </c>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>5</v>
@@ -985,47 +1100,53 @@
         <v>10</v>
       </c>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>5</v>
@@ -1034,13 +1155,15 @@
         <v>10</v>
       </c>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>5</v>
@@ -1049,13 +1172,15 @@
         <v>10</v>
       </c>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>2</v>
@@ -1064,13 +1189,17 @@
       <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>2</v>
@@ -1079,13 +1208,19 @@
       <c r="E28" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>5</v>
@@ -1094,103 +1229,158 @@
         <v>10</v>
       </c>
       <c r="E29" s="4"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>